<commit_message>
MHLM RNAV (GNSS) RWY 22
Update
</commit_message>
<xml_diff>
--- a/03_AD/MHLM/MHLM_RNAV_TABLES.xlsx
+++ b/03_AD/MHLM/MHLM_RNAV_TABLES.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18120" windowHeight="10740" tabRatio="599" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18120" windowHeight="10740" tabRatio="599" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MHLM STAR RNP2 RWY 22" sheetId="10" r:id="rId1"/>
-    <sheet name="MHLM RNAV SID RWY 04" sheetId="11" r:id="rId2"/>
+    <sheet name="MHLM SID RNP2 RWY 04" sheetId="11" r:id="rId2"/>
+    <sheet name="MHLM RNAV GNSS RWY22" sheetId="12" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'MHLM STAR RNP2 RWY 22'!$A$1:$M$5</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="134">
   <si>
     <t>-</t>
   </si>
@@ -336,6 +337,105 @@
   </si>
   <si>
     <t>56.30 NM</t>
+  </si>
+  <si>
+    <t>Waypoint
+Identifier</t>
+  </si>
+  <si>
+    <t>VPA(°)/
+ TCH (ft)</t>
+  </si>
+  <si>
+    <t>Navigation
+Specification</t>
+  </si>
+  <si>
+    <t>RNP APCH</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>-3°/50'</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>D/d</t>
+  </si>
+  <si>
+    <t>M/d</t>
+  </si>
+  <si>
+    <t>DECLINATION</t>
+  </si>
+  <si>
+    <t>IAF LM001</t>
+  </si>
+  <si>
+    <t>IAF LM003</t>
+  </si>
+  <si>
+    <t>0º14'W</t>
+  </si>
+  <si>
+    <t>LM002</t>
+  </si>
+  <si>
+    <t>LM008</t>
+  </si>
+  <si>
+    <t>RWY22</t>
+  </si>
+  <si>
+    <t>LM011</t>
+  </si>
+  <si>
+    <t>+ 5587</t>
+  </si>
+  <si>
+    <t>+ 666</t>
+  </si>
+  <si>
+    <t>0874654.20W</t>
+  </si>
+  <si>
+    <t>153207.13N</t>
+  </si>
+  <si>
+    <t>0875104.71W</t>
+  </si>
+  <si>
+    <t>152741.89053N</t>
+  </si>
+  <si>
+    <t>0875456.53047W</t>
+  </si>
+  <si>
+    <t>152540.90N</t>
+  </si>
+  <si>
+    <t>0875642.28W</t>
+  </si>
+  <si>
+    <t>153653.36N</t>
+  </si>
+  <si>
+    <t>0º16'W</t>
+  </si>
+  <si>
+    <t>0º13'W</t>
+  </si>
+  <si>
+    <t>0º09'W</t>
+  </si>
+  <si>
+    <t>0º22'W</t>
   </si>
 </sst>
 </file>
@@ -345,7 +445,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,8 +490,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,8 +529,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -457,11 +582,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -512,6 +646,60 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2003,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3017,4 +3205,1023 @@
     <ignoredError sqref="I19 I14 I9 I4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="12" max="12" width="8.875" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+    </row>
+    <row r="2" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" s="37"/>
+      <c r="O2" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="R2" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+    </row>
+    <row r="3" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="34">
+        <v>8000</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="37"/>
+      <c r="O3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="24" t="str">
+        <f>T4</f>
+        <v>157.2 (157.0)</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="34">
+        <v>4000</v>
+      </c>
+      <c r="I4" s="36">
+        <v>13.23</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" s="37"/>
+      <c r="O4" s="32">
+        <v>156.99593400000001</v>
+      </c>
+      <c r="P4" s="31" t="str">
+        <f>MID(K3,1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="31" t="str">
+        <f>MID(K3,3,2)</f>
+        <v>14</v>
+      </c>
+      <c r="R4" s="31">
+        <f>-(P4+Q4/60)</f>
+        <v>-0.23333333333333334</v>
+      </c>
+      <c r="S4" s="31">
+        <f>O4-R4</f>
+        <v>157.22926733333333</v>
+      </c>
+      <c r="T4" s="31" t="str">
+        <f>TEXT(S4,"000.0")&amp;TEXT(O4," (000.0)")</f>
+        <v>157.2 (157.0)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="24" t="str">
+        <f t="shared" ref="F5:F8" si="0">T5</f>
+        <v>220.6 (220.3)</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="34">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="36">
+        <v>6.23</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" s="37"/>
+      <c r="O5" s="32">
+        <v>220.31860599999999</v>
+      </c>
+      <c r="P5" s="31" t="str">
+        <f t="shared" ref="P5:P8" si="1">MID(K4,1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="31" t="str">
+        <f t="shared" ref="Q5:Q8" si="2">MID(K4,3,2)</f>
+        <v>16</v>
+      </c>
+      <c r="R5" s="31">
+        <f>-(P5+Q5/60)</f>
+        <v>-0.26666666666666666</v>
+      </c>
+      <c r="S5" s="31">
+        <f t="shared" ref="S5:S8" si="3">O5-R5</f>
+        <v>220.58527266666667</v>
+      </c>
+      <c r="T5" s="31" t="str">
+        <f t="shared" ref="T5:T8" si="4">TEXT(S5,"000.0")&amp;TEXT(O5," (000.0)")</f>
+        <v>220.6 (220.3)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>220.5 (220.3)</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="34">
+        <v>135</v>
+      </c>
+      <c r="I6" s="36">
+        <v>5.77</v>
+      </c>
+      <c r="J6" s="24">
+        <v>165</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N6" s="37"/>
+      <c r="O6" s="32">
+        <v>220.28969699999999</v>
+      </c>
+      <c r="P6" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="R6" s="31">
+        <f>-(P6+Q6/60)</f>
+        <v>-0.21666666666666667</v>
+      </c>
+      <c r="S6" s="31">
+        <f t="shared" si="3"/>
+        <v>220.50636366666666</v>
+      </c>
+      <c r="T6" s="31" t="str">
+        <f t="shared" si="4"/>
+        <v>220.5 (220.3)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>220.4 (220.3)</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" s="36">
+        <v>2.63</v>
+      </c>
+      <c r="J7" s="24">
+        <v>265</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N7" s="37"/>
+      <c r="O7" s="32">
+        <v>220.29329000000001</v>
+      </c>
+      <c r="P7" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>09</v>
+      </c>
+      <c r="R7" s="31">
+        <f>-(P7+Q7/60)</f>
+        <v>-0.15</v>
+      </c>
+      <c r="S7" s="31">
+        <f t="shared" si="3"/>
+        <v>220.44329000000002</v>
+      </c>
+      <c r="T7" s="31" t="str">
+        <f t="shared" si="4"/>
+        <v>220.4 (220.3)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>171.8 (171.7)</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="I8" s="36">
+        <v>19.27</v>
+      </c>
+      <c r="J8" s="24">
+        <v>265</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N8" s="37"/>
+      <c r="O8" s="32">
+        <v>171.65588099999999</v>
+      </c>
+      <c r="P8" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>09</v>
+      </c>
+      <c r="R8" s="31">
+        <f>-(P8+Q8/60)</f>
+        <v>-0.15</v>
+      </c>
+      <c r="S8" s="31">
+        <f t="shared" si="3"/>
+        <v>171.805881</v>
+      </c>
+      <c r="T8" s="31" t="str">
+        <f t="shared" si="4"/>
+        <v>171.8 (171.7)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="33"/>
+    </row>
+    <row r="10" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+    </row>
+    <row r="11" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="N11" s="37"/>
+      <c r="O11" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="P11" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q11" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="R11" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+    </row>
+    <row r="12" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="34">
+        <v>7100</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N12" s="37"/>
+      <c r="O12" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" s="31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="24" t="str">
+        <f>T13</f>
+        <v>308.8 (308.4)</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13" s="34">
+        <v>4000</v>
+      </c>
+      <c r="I13" s="36">
+        <v>17.739999999999998</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N13" s="37"/>
+      <c r="O13" s="32">
+        <v>308.426106</v>
+      </c>
+      <c r="P13" s="31" t="str">
+        <f>MID(K12,1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="31" t="str">
+        <f>MID(K12,3,2)</f>
+        <v>22</v>
+      </c>
+      <c r="R13" s="31">
+        <f>-(P13+Q13/60)</f>
+        <v>-0.36666666666666664</v>
+      </c>
+      <c r="S13" s="31">
+        <f>O13-R13</f>
+        <v>308.79277266666668</v>
+      </c>
+      <c r="T13" s="31" t="str">
+        <f>TEXT(S13,"000.0")&amp;TEXT(O13," (000.0)")</f>
+        <v>308.8 (308.4)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="24" t="str">
+        <f t="shared" ref="F14:F17" si="5">T14</f>
+        <v>220.6 (220.3)</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="34">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="36">
+        <v>6.23</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N14" s="37"/>
+      <c r="O14" s="32">
+        <v>220.31860599999999</v>
+      </c>
+      <c r="P14" s="31" t="str">
+        <f t="shared" ref="P14:P17" si="6">MID(K13,1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="31" t="str">
+        <f t="shared" ref="Q14:Q17" si="7">MID(K13,3,2)</f>
+        <v>16</v>
+      </c>
+      <c r="R14" s="31">
+        <f>-(P14+Q14/60)</f>
+        <v>-0.26666666666666666</v>
+      </c>
+      <c r="S14" s="31">
+        <f t="shared" ref="S14:S17" si="8">O14-R14</f>
+        <v>220.58527266666667</v>
+      </c>
+      <c r="T14" s="31" t="str">
+        <f t="shared" ref="T14:T17" si="9">TEXT(S14,"000.0")&amp;TEXT(O14," (000.0)")</f>
+        <v>220.6 (220.3)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>220.5 (220.3)</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="34">
+        <v>135</v>
+      </c>
+      <c r="I15" s="36">
+        <v>5.77</v>
+      </c>
+      <c r="J15" s="24">
+        <v>165</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" s="37"/>
+      <c r="O15" s="32">
+        <v>220.28969699999999</v>
+      </c>
+      <c r="P15" s="31" t="str">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="31" t="str">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="R15" s="31">
+        <f>-(P15+Q15/60)</f>
+        <v>-0.21666666666666667</v>
+      </c>
+      <c r="S15" s="31">
+        <f t="shared" si="8"/>
+        <v>220.50636366666666</v>
+      </c>
+      <c r="T15" s="31" t="str">
+        <f t="shared" si="9"/>
+        <v>220.5 (220.3)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>220.4 (220.3)</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="I16" s="36">
+        <v>2.63</v>
+      </c>
+      <c r="J16" s="24">
+        <v>265</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N16" s="37"/>
+      <c r="O16" s="32">
+        <v>220.29329000000001</v>
+      </c>
+      <c r="P16" s="31" t="str">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="31" t="str">
+        <f t="shared" si="7"/>
+        <v>09</v>
+      </c>
+      <c r="R16" s="31">
+        <f>-(P16+Q16/60)</f>
+        <v>-0.15</v>
+      </c>
+      <c r="S16" s="31">
+        <f t="shared" si="8"/>
+        <v>220.44329000000002</v>
+      </c>
+      <c r="T16" s="31" t="str">
+        <f t="shared" si="9"/>
+        <v>220.4 (220.3)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>171.8 (171.7)</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="I17" s="36">
+        <v>19.27</v>
+      </c>
+      <c r="J17" s="24">
+        <v>265</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N17" s="37"/>
+      <c r="O17" s="32">
+        <v>171.65588099999999</v>
+      </c>
+      <c r="P17" s="31" t="str">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="31" t="str">
+        <f t="shared" si="7"/>
+        <v>09</v>
+      </c>
+      <c r="R17" s="31">
+        <f>-(P17+Q17/60)</f>
+        <v>-0.15</v>
+      </c>
+      <c r="S17" s="31">
+        <f t="shared" si="8"/>
+        <v>171.805881</v>
+      </c>
+      <c r="T17" s="31" t="str">
+        <f t="shared" si="9"/>
+        <v>171.8 (171.7)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="37"/>
+    </row>
+    <row r="19" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="N19" s="37"/>
+    </row>
+    <row r="20" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="N20" s="37"/>
+    </row>
+    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="N21" s="37"/>
+    </row>
+    <row r="22" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="N22" s="37"/>
+    </row>
+    <row r="23" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="N23" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="H7:H8 H16:H17" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>